<commit_message>
Assigner and test_experiment with prompting for Self-Defined bins: assignByPc implemented but not tested on subjects
</commit_message>
<xml_diff>
--- a/biasweb/utils/data/SampleExpData_oneSheet.xlsx
+++ b/biasweb/utils/data/SampleExpData_oneSheet.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\biasweb\test_scripts\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\biasweb.dev\biasweb\utils\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -80,7 +80,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -423,7 +423,7 @@
   <dimension ref="A1:C49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -455,7 +455,7 @@
         <v>16010073</v>
       </c>
       <c r="B3" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C3" t="s">
         <v>1</v>
@@ -466,7 +466,7 @@
         <v>16010074</v>
       </c>
       <c r="B4" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C4" t="s">
         <v>1</v>
@@ -488,7 +488,7 @@
         <v>16010005</v>
       </c>
       <c r="B6" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C6" t="s">
         <v>3</v>
@@ -906,7 +906,7 @@
         <v>16010061</v>
       </c>
       <c r="B44" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C44" t="s">
         <v>12</v>
@@ -917,7 +917,7 @@
         <v>16010078</v>
       </c>
       <c r="B45" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C45" t="s">
         <v>12</v>
@@ -939,7 +939,7 @@
         <v>16010057</v>
       </c>
       <c r="B47" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C47" t="s">
         <v>13</v>
@@ -961,7 +961,7 @@
         <v>16010075</v>
       </c>
       <c r="B49" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C49" t="s">
         <v>13</v>

</xml_diff>